<commit_message>
warehouse with entry processes recording test coded
</commit_message>
<xml_diff>
--- a/soberano/test_cases/process_record_test_cases.xlsx
+++ b/soberano/test_cases/process_record_test_cases.xlsx
@@ -124,7 +124,7 @@
     <t xml:space="preserve">User18 is NOT allowed to record process</t>
   </si>
   <si>
-    <t xml:space="preserve">pr91</t>
+    <t xml:space="preserve">pr10</t>
   </si>
   <si>
     <t xml:space="preserve">User19 is allowed to record process</t>
@@ -133,7 +133,7 @@
     <t xml:space="preserve">User20 is NOT allowed to record process</t>
   </si>
   <si>
-    <t xml:space="preserve">pr92</t>
+    <t xml:space="preserve">pr11</t>
   </si>
   <si>
     <t xml:space="preserve">User21 is NOT allowed to record process</t>
@@ -169,7 +169,7 @@
     <t xml:space="preserve">check pr9 data is correctly shown in details panel</t>
   </si>
   <si>
-    <t xml:space="preserve">check pr91 data is correctly shown in details panel</t>
+    <t xml:space="preserve">check pr10 data is correctly shown in details panel</t>
   </si>
 </sst>
 </file>
@@ -314,8 +314,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ36"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A37" activeCellId="0" sqref="A37"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B36" activeCellId="0" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -642,7 +642,7 @@
         <v>34</v>
       </c>
       <c r="D22" s="2" t="n">
-        <v>91</v>
+        <v>10</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -656,7 +656,7 @@
         <v>34</v>
       </c>
       <c r="D23" s="2" t="n">
-        <v>91</v>
+        <v>10</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -670,7 +670,7 @@
         <v>37</v>
       </c>
       <c r="D24" s="2" t="n">
-        <v>92</v>
+        <v>11</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -684,7 +684,7 @@
         <v>37</v>
       </c>
       <c r="D25" s="2" t="n">
-        <v>92</v>
+        <v>11</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -698,7 +698,7 @@
         <v>34</v>
       </c>
       <c r="D26" s="2" t="n">
-        <v>91</v>
+        <v>10</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>